<commit_message>
Finished visitWebsite and editCompetition
</commit_message>
<xml_diff>
--- a/storage.xlsx
+++ b/storage.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="testing competition #1" r:id="rId3" sheetId="1"/>
+    <sheet name="Name" r:id="rId3" sheetId="1"/>
     <sheet name="testing competition #2" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
@@ -18,7 +18,7 @@
     <t>Competition Name</t>
   </si>
   <si>
-    <t>testing competition #1</t>
+    <t>Name</t>
   </si>
   <si>
     <t>Competition Link</t>
@@ -159,7 +159,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="18.0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.265625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.24609375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.90625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.11328125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.44140625" customWidth="true" bestFit="true"/>
@@ -186,7 +186,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n" s="1">
-        <v>44533.0</v>
+        <v>44551.0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
complete validation for all input dialogs
</commit_message>
<xml_diff>
--- a/storage.xlsx
+++ b/storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\KFUPM Vault\211\SWE206\Project\Phase Three\test-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2E3A9E-189E-45ED-919E-E67ABF59C5D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295718BC-7FEA-406A-A4E1-28B9282BBD89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testing competition #1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>Competition Link</t>
   </si>
   <si>
-    <t>http://cheeks</t>
-  </si>
-  <si>
     <t>Competition Date</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>https://twitter.com</t>
+  </si>
+  <si>
+    <t>https://reddit.com</t>
   </si>
 </sst>
 </file>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,12 +504,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>44533</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -525,19 +525,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -545,13 +545,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -562,16 +562,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -579,16 +579,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -596,16 +596,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -613,33 +613,33 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -647,13 +647,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -664,16 +664,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -681,16 +681,16 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -698,16 +698,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -715,33 +715,33 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -756,7 +756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -772,20 +774,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>44533</v>
@@ -793,7 +795,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -801,19 +803,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -821,13 +823,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -838,16 +840,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -855,16 +857,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -872,16 +874,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -889,33 +891,33 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -923,13 +925,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -940,16 +942,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -957,16 +959,16 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -974,16 +976,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -991,36 +993,39 @@
         <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{162FB4B9-BF58-417E-8A96-63BF32861853}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tested `ExcelStorage.java` and `MainController.java`
</commit_message>
<xml_diff>
--- a/storage.xlsx
+++ b/storage.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\KFUPM Vault\211\SWE206\Project\Phase Three\test-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295718BC-7FEA-406A-A4E1-28B9282BBD89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868A5AB9-3F9A-4E8F-977D-601E41C33DDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testing competition #1" sheetId="1" r:id="rId1"/>
     <sheet name="testing competition #2" sheetId="2" r:id="rId2"/>
+    <sheet name="testing competition #3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="32">
   <si>
     <t>Competition Name</t>
   </si>
@@ -32,6 +33,9 @@
     <t>Competition Link</t>
   </si>
   <si>
+    <t>http://cheeks</t>
+  </si>
+  <si>
     <t>Competition Date</t>
   </si>
   <si>
@@ -89,31 +93,41 @@
     <t>Abdulaziz</t>
   </si>
   <si>
+    <t>Muhab Abubaker</t>
+  </si>
+  <si>
+    <t>Ahmed Badghaish</t>
+  </si>
+  <si>
+    <t>Basel Al nassr</t>
+  </si>
+  <si>
+    <t>Mubarak Badgaish</t>
+  </si>
+  <si>
+    <t>Abdulaziz bin Agian</t>
+  </si>
+  <si>
+    <t>201945575</t>
+  </si>
+  <si>
+    <t>Kermit the frog</t>
+  </si>
+  <si>
     <t>testing competition #2</t>
   </si>
   <si>
-    <t>https://twitter.com</t>
-  </si>
-  <si>
-    <t>https://reddit.com</t>
+    <t>testing competition #3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,19 +165,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,15 +489,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -503,21 +512,21 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>23</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>44533</v>
+        <v>44541</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -525,19 +534,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -545,13 +554,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -562,16 +571,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -579,16 +588,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -596,16 +605,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -613,33 +622,33 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -647,16 +656,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -664,16 +673,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -681,16 +690,16 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -698,16 +707,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -715,39 +724,36 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
+      <c r="A18" s="2">
+        <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F3951DD5-C9F3-462E-9E23-4C7B8789A76B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -756,15 +762,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -774,28 +780,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>44533</v>
+        <v>44541</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -803,19 +809,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -823,13 +829,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -840,16 +846,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -857,16 +863,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -874,16 +880,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -891,33 +897,33 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -925,16 +931,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -942,16 +948,16 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -959,16 +965,16 @@
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -976,16 +982,16 @@
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -993,39 +999,307 @@
         <v>10</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340F2921-43AC-47E0-99E4-48BFDCA7897B}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>15</v>
+      <c r="A18" s="3">
+        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{162FB4B9-BF58-417E-8A96-63BF32861853}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalized version of the code
</commit_message>
<xml_diff>
--- a/storage.xlsx
+++ b/storage.xlsx
@@ -6,24 +6,24 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="competition a" r:id="rId3" sheetId="1"/>
+    <sheet name="EG" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Competition Name</t>
   </si>
   <si>
-    <t>competition a</t>
+    <t>EG</t>
   </si>
   <si>
     <t>Competition Link</t>
   </si>
   <si>
-    <t>https://reddit.com</t>
+    <t>https://noon.com</t>
   </si>
   <si>
     <t>Competition Date</t>
@@ -45,27 +45,6 @@
   </si>
   <si>
     <t>Rank</t>
-  </si>
-  <si>
-    <t>201945570</t>
-  </si>
-  <si>
-    <t>st a</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>201945571</t>
-  </si>
-  <si>
-    <t>st b</t>
-  </si>
-  <si>
-    <t>SWE</t>
   </si>
 </sst>
 </file>
@@ -132,14 +111,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="18.0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="17.7890625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.0078125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.90625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="6.42578125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.44140625" customWidth="true" bestFit="true"/>
@@ -166,7 +145,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n" s="1">
-        <v>44547.0</v>
+        <v>44553.0</v>
       </c>
     </row>
     <row r="4">
@@ -174,7 +153,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="6">
@@ -194,40 +173,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>